<commit_message>
Back to work on tooltips. Some done. Some not. Some not working. SS
</commit_message>
<xml_diff>
--- a/Tooltips.xlsx
+++ b/Tooltips.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>The goal is to run .tooltip on each selected DOM element only once.</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>When the index page is first displayed, the TypeWell "surrounding" items should all be selectable at once for tooltip activation.</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>need image name</t>
   </si>
 </sst>
 </file>
@@ -83,8 +89,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,73 +377,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B10"/>
+  <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>